<commit_message>
button reporting system utils get mail and password for testing news optimization
</commit_message>
<xml_diff>
--- a/ReportingSystem/Users.xlsx
+++ b/ReportingSystem/Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - ДІДЖИТАП,ТОВ\.NET\Diplom\Project\ReportingSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD940549-D536-4833-961C-BD44DF0D2A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8BC658-43C0-4707-A169-11B2A48A870A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16905" yWindow="9900" windowWidth="14925" windowHeight="11805" xr2:uid="{4C2A6DE6-1079-4474-97BA-3339B0708E36}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="23">
   <si>
     <t>EUDeveloper</t>
   </si>
@@ -461,7 +461,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,6 +754,9 @@
       <c r="N7" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="O7" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -775,6 +778,9 @@
         <v>10</v>
       </c>
       <c r="M8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>